<commit_message>
ATL15_output_attrs: fixed some typos, added source and long name fields
</commit_message>
<xml_diff>
--- a/ATL15_output_attrs.xlsx
+++ b/ATL15_output_attrs.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/git_repos/surfacechange/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{300448D2-BD6B-4E43-9975-6A5A596B67FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD5616C-7BF9-2641-A0A2-41B9B7652DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="980" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="300" yWindow="4380" windowWidth="32300" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ATL15_output_attrs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="210">
   <si>
     <t>group</t>
   </si>
@@ -400,9 +400,6 @@
     <t>y coordinate of the 20-km cell centers, in projected coordinates</t>
   </si>
   <si>
-    <t>Fraction of the 20x20 km cell identified as ice in the ATL14 ice mask</t>
-  </si>
-  <si>
     <t>20x20 km average height change relative to the datum (Jan 1, 2020) surface</t>
   </si>
   <si>
@@ -430,9 +427,6 @@
     <t>y coordinate of the 40-km cell centers, in projected coordinates</t>
   </si>
   <si>
-    <t>Fraction of the 40x40 km cell identified as ice in the ATL14 ice mask</t>
-  </si>
-  <si>
     <t>40x40 km average height change relative to the datum (Jan 1, 4040) surface</t>
   </si>
   <si>
@@ -451,12 +445,6 @@
     <t>Uncertainty in the 40x40 km average annual height change rate</t>
   </si>
   <si>
-    <t>ice_mask_fraction_20km</t>
-  </si>
-  <si>
-    <t>ice_mask_fraction_40km</t>
-  </si>
-  <si>
     <t>Time for the midpoint of each biennial height-change rate</t>
   </si>
   <si>
@@ -500,13 +488,175 @@
   </si>
   <si>
     <t>Ice-covered area of each 40x40 km grid cell, accounting for the area distortion in the polar-stereographic projections</t>
+  </si>
+  <si>
+    <t>quarterly h(t) time</t>
+  </si>
+  <si>
+    <t>quarterly dh/dt time</t>
+  </si>
+  <si>
+    <t>annual dh/dt time</t>
+  </si>
+  <si>
+    <t>biennial dh/dt time</t>
+  </si>
+  <si>
+    <t>polar stereographic x at 1km</t>
+  </si>
+  <si>
+    <t>polar stereographic y at 1km</t>
+  </si>
+  <si>
+    <t>cell area at 1 km</t>
+  </si>
+  <si>
+    <t>Ice mask at 1km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rms misfit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data count </t>
+  </si>
+  <si>
+    <t>scaled rms misfit</t>
+  </si>
+  <si>
+    <t>quarterly height-change rate at 1 km</t>
+  </si>
+  <si>
+    <t>quarterly height-change rate uncertainty at 1 km</t>
+  </si>
+  <si>
+    <t>annual height-change rate at 1 km</t>
+  </si>
+  <si>
+    <t>annual height-change rate uncertainty at 1 km</t>
+  </si>
+  <si>
+    <t>biennial height-change rate at 1 km</t>
+  </si>
+  <si>
+    <t>biennial height-change rate uncertainty at 1 km</t>
+  </si>
+  <si>
+    <t>polar stereographic x at 10 km</t>
+  </si>
+  <si>
+    <t>polar stereographic y at 10 km</t>
+  </si>
+  <si>
+    <t>quarterly height change  at 1 km</t>
+  </si>
+  <si>
+    <t>quarterly height change uncertainty at 1 km</t>
+  </si>
+  <si>
+    <t>ice covered area at 10 km</t>
+  </si>
+  <si>
+    <t>quarterly height change  at 10 km</t>
+  </si>
+  <si>
+    <t>quarterly height change uncertainty at 10 km</t>
+  </si>
+  <si>
+    <t>quarterly height-change rate at 10 km</t>
+  </si>
+  <si>
+    <t>quarterly height-change rate uncertainty at 10 km</t>
+  </si>
+  <si>
+    <t>annual height-change rate at 10 km</t>
+  </si>
+  <si>
+    <t>annual height-change rate uncertainty at 10 km</t>
+  </si>
+  <si>
+    <t>biennial height-change rate at 10 km</t>
+  </si>
+  <si>
+    <t>biennial height-change rate uncertainty at 10 km</t>
+  </si>
+  <si>
+    <t>polar stereographic y at 20 km</t>
+  </si>
+  <si>
+    <t>ice covered area at 20 km</t>
+  </si>
+  <si>
+    <t>quarterly height change  at 20 km</t>
+  </si>
+  <si>
+    <t>quarterly height change uncertainty at 20 km</t>
+  </si>
+  <si>
+    <t>quarterly height-change rate at 20 km</t>
+  </si>
+  <si>
+    <t>quarterly height-change rate uncertainty at 20 km</t>
+  </si>
+  <si>
+    <t>annual height-change rate at 20 km</t>
+  </si>
+  <si>
+    <t>annual height-change rate uncertainty at 20 km</t>
+  </si>
+  <si>
+    <t>biennial height-change rate at 20 km</t>
+  </si>
+  <si>
+    <t>biennial height-change rate uncertainty at 20 km</t>
+  </si>
+  <si>
+    <t>polar stereographic x at 20 km</t>
+  </si>
+  <si>
+    <t>polar stereographic x at 40 km</t>
+  </si>
+  <si>
+    <t>polar stereographic y at 40 km</t>
+  </si>
+  <si>
+    <t>ice covered area at 40 km</t>
+  </si>
+  <si>
+    <t>quarterly height change  at 40 km</t>
+  </si>
+  <si>
+    <t>quarterly height change uncertainty at 40 km</t>
+  </si>
+  <si>
+    <t>quarterly height-change rate at 40 km</t>
+  </si>
+  <si>
+    <t>quarterly height-change rate uncertainty at 40 km</t>
+  </si>
+  <si>
+    <t>annual height-change rate at 40 km</t>
+  </si>
+  <si>
+    <t>annual height-change rate uncertainty at 40 km</t>
+  </si>
+  <si>
+    <t>biennial height-change rate at 40 km</t>
+  </si>
+  <si>
+    <t>biennial height-change rate uncertainty at 40 km</t>
+  </si>
+  <si>
+    <t>3.3.2</t>
+  </si>
+  <si>
+    <t>5.2.4.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -641,6 +791,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -823,7 +980,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -938,6 +1095,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -983,8 +1149,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1339,11 +1510,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1351,36 +1522,38 @@
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="58.33203125" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1406,6 +1579,9 @@
       <c r="G2" t="s">
         <v>93</v>
       </c>
+      <c r="H2" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1424,10 +1600,13 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
         <v>122</v>
+      </c>
+      <c r="H3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1452,13 +1631,16 @@
       <c r="G4" t="s">
         <v>121</v>
       </c>
+      <c r="H4" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1473,7 +1655,10 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>145</v>
+        <v>141</v>
+      </c>
+      <c r="H5" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1498,6 +1683,12 @@
       <c r="G7" t="s">
         <v>106</v>
       </c>
+      <c r="H7" t="s">
+        <v>160</v>
+      </c>
+      <c r="I7" s="2">
+        <v>3.2</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1521,6 +1712,12 @@
       <c r="G8" t="s">
         <v>107</v>
       </c>
+      <c r="H8" t="s">
+        <v>161</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3.2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1542,7 +1739,13 @@
         <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>156</v>
+        <v>152</v>
+      </c>
+      <c r="H9" t="s">
+        <v>162</v>
+      </c>
+      <c r="I9" s="2">
+        <v>3.4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1559,13 +1762,19 @@
         <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F10" t="s">
         <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>154</v>
+        <v>150</v>
+      </c>
+      <c r="H10" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1590,6 +1799,12 @@
       <c r="G11" t="s">
         <v>94</v>
       </c>
+      <c r="H11" t="s">
+        <v>165</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1613,6 +1828,12 @@
       <c r="G12" t="s">
         <v>95</v>
       </c>
+      <c r="H12" t="s">
+        <v>164</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1636,6 +1857,12 @@
       <c r="G13" t="s">
         <v>96</v>
       </c>
+      <c r="H13" t="s">
+        <v>166</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1659,6 +1886,12 @@
       <c r="G14" t="s">
         <v>97</v>
       </c>
+      <c r="H14" t="s">
+        <v>175</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1682,6 +1915,12 @@
       <c r="G15" t="s">
         <v>98</v>
       </c>
+      <c r="H15" t="s">
+        <v>176</v>
+      </c>
+      <c r="I15" s="2">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1705,8 +1944,14 @@
       <c r="G16" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>167</v>
+      </c>
+      <c r="I16" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1728,8 +1973,14 @@
       <c r="G17" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>168</v>
+      </c>
+      <c r="I17" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1751,8 +2002,14 @@
       <c r="G18" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>169</v>
+      </c>
+      <c r="I18" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1774,8 +2031,14 @@
       <c r="G19" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>170</v>
+      </c>
+      <c r="I19" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1795,10 +2058,16 @@
         <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I20" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1818,10 +2087,16 @@
         <v>28</v>
       </c>
       <c r="G21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I21" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1843,8 +2118,14 @@
       <c r="G23" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I23" s="2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1866,8 +2147,14 @@
       <c r="G24" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>174</v>
+      </c>
+      <c r="I24" s="2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1887,10 +2174,16 @@
         <v>28</v>
       </c>
       <c r="G25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="H25" t="s">
+        <v>177</v>
+      </c>
+      <c r="I25" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1912,8 +2205,14 @@
       <c r="G26" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>178</v>
+      </c>
+      <c r="I26" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1935,8 +2234,14 @@
       <c r="G27" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>179</v>
+      </c>
+      <c r="I27" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -1958,8 +2263,14 @@
       <c r="G28" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>180</v>
+      </c>
+      <c r="I28" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1981,8 +2292,14 @@
       <c r="G29" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>181</v>
+      </c>
+      <c r="I29" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -2004,8 +2321,14 @@
       <c r="G30" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>182</v>
+      </c>
+      <c r="I30" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -2027,8 +2350,14 @@
       <c r="G31" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>183</v>
+      </c>
+      <c r="I31" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -2048,10 +2377,16 @@
         <v>119</v>
       </c>
       <c r="G32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I32" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2071,10 +2406,16 @@
         <v>119</v>
       </c>
       <c r="G33" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I33" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -2094,10 +2435,16 @@
         <v>28</v>
       </c>
       <c r="G35" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="H35" t="s">
+        <v>196</v>
+      </c>
+      <c r="I35" s="2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2119,8 +2466,14 @@
       <c r="G36" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>186</v>
+      </c>
+      <c r="I36" s="2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -2140,41 +2493,53 @@
         <v>28</v>
       </c>
       <c r="G37" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="H37" t="s">
+        <v>187</v>
+      </c>
+      <c r="I37" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>63</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E38" t="s">
         <v>27</v>
       </c>
       <c r="F38" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="G38" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>188</v>
+      </c>
+      <c r="I38" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C39" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
         <v>64</v>
@@ -2188,36 +2553,48 @@
       <c r="G39" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>189</v>
+      </c>
+      <c r="I39" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
         <v>27</v>
       </c>
       <c r="F40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G40" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>190</v>
+      </c>
+      <c r="I40" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C41" t="s">
         <v>37</v>
@@ -2234,36 +2611,48 @@
       <c r="G41" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>191</v>
+      </c>
+      <c r="I41" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
         <v>37</v>
       </c>
       <c r="D42" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E42" t="s">
         <v>27</v>
       </c>
       <c r="F42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G42" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>192</v>
+      </c>
+      <c r="I42" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
         <v>37</v>
@@ -2280,36 +2669,48 @@
       <c r="G43" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>193</v>
+      </c>
+      <c r="I43" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
         <v>37</v>
       </c>
       <c r="D44" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E44" t="s">
         <v>27</v>
       </c>
       <c r="F44" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="G44" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I44" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C45" t="s">
         <v>37</v>
@@ -2324,44 +2725,56 @@
         <v>119</v>
       </c>
       <c r="G45" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" t="s">
-        <v>124</v>
-      </c>
-      <c r="C46" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" t="s">
-        <v>62</v>
-      </c>
-      <c r="E46" t="s">
-        <v>27</v>
-      </c>
-      <c r="F46" t="s">
-        <v>119</v>
-      </c>
-      <c r="G46" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I45" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47" t="s">
+        <v>133</v>
+      </c>
+      <c r="H47" t="s">
+        <v>197</v>
+      </c>
+      <c r="I47" s="2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C48" t="s">
         <v>20</v>
       </c>
       <c r="D48" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -2372,258 +2785,272 @@
       <c r="G48" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>198</v>
+      </c>
+      <c r="I48" s="2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F49" t="s">
         <v>28</v>
       </c>
       <c r="G49" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="H49" t="s">
+        <v>199</v>
+      </c>
+      <c r="I49" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>72</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E50" t="s">
         <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="G50" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="H50" t="s">
+        <v>200</v>
+      </c>
+      <c r="I50" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>72</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="C51" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D51" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E51" t="s">
         <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="G51" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>201</v>
+      </c>
+      <c r="I51" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>72</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D52" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E52" t="s">
         <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G52" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>202</v>
+      </c>
+      <c r="I52" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>72</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C53" t="s">
         <v>37</v>
       </c>
       <c r="D53" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E53" t="s">
         <v>27</v>
       </c>
       <c r="F53" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G53" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>203</v>
+      </c>
+      <c r="I53" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>72</v>
       </c>
       <c r="B54" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C54" t="s">
         <v>37</v>
       </c>
       <c r="D54" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E54" t="s">
         <v>27</v>
       </c>
       <c r="F54" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G54" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
+        <v>204</v>
+      </c>
+      <c r="I54" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>72</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C55" t="s">
         <v>37</v>
       </c>
       <c r="D55" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E55" t="s">
         <v>27</v>
       </c>
       <c r="F55" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G55" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>205</v>
+      </c>
+      <c r="I55" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C56" t="s">
         <v>37</v>
       </c>
       <c r="D56" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E56" t="s">
         <v>27</v>
       </c>
       <c r="F56" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="G56" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I56" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>72</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C57" t="s">
         <v>37</v>
       </c>
       <c r="D57" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E57" t="s">
         <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="G57" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" t="s">
-        <v>88</v>
-      </c>
-      <c r="C58" t="s">
-        <v>37</v>
-      </c>
-      <c r="D58" t="s">
-        <v>78</v>
-      </c>
-      <c r="E58" t="s">
-        <v>27</v>
-      </c>
-      <c r="F58" t="s">
-        <v>119</v>
-      </c>
-      <c r="G58" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>72</v>
-      </c>
-      <c r="B59" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" t="s">
-        <v>37</v>
-      </c>
-      <c r="D59" t="s">
-        <v>78</v>
-      </c>
-      <c r="E59" t="s">
-        <v>27</v>
-      </c>
-      <c r="F59" t="s">
-        <v>119</v>
-      </c>
-      <c r="G59" t="s">
-        <v>153</v>
+        <v>149</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I57" s="2">
+        <v>3.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>